<commit_message>
Update displayed press brands
</commit_message>
<xml_diff>
--- a/mapa_adresy_pbc.xlsx
+++ b/mapa_adresy_pbc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapto\OneDrive\Pulpit\Social-Media\Social-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE7BFA4-9F93-4FE2-9335-F5D8CC9D3865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58A08B9-B115-445C-AEE1-F90BB72B1C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="305">
   <si>
     <t>Tytuł</t>
   </si>
@@ -537,9 +537,6 @@
     <t>https://www.pbc.pl/badany-tytul/zwierciadlo/</t>
   </si>
   <si>
-    <t>https://www.pbc.pl/badany-tytul/sprawny-marketing/</t>
-  </si>
-  <si>
     <t>https://www.pbc.pl/badany-tytul/tele-magazyn/</t>
   </si>
   <si>
@@ -657,9 +654,6 @@
     <t>https://www.pbc.pl/badany-tytul/automobilista/</t>
   </si>
   <si>
-    <t>https://www.pbc.pl/badany-tytul/sport/</t>
-  </si>
-  <si>
     <t>https://www.pbc.pl/badany-tytul/gazeta-podatkowa/</t>
   </si>
   <si>
@@ -753,9 +747,6 @@
     <t>https://www.pbc.pl/badany-tytul/swierszczyk/</t>
   </si>
   <si>
-    <t>https://www.pbc.pl/badany-tytul/super-nowosci/</t>
-  </si>
-  <si>
     <t>https://www.pbc.pl/badany-tytul/lego-city/</t>
   </si>
   <si>
@@ -787,9 +778,6 @@
   </si>
   <si>
     <t>https://www.pbc.pl/badany-tytul/inzynier-budownictwa/</t>
-  </si>
-  <si>
-    <t>https://www.pbc.pl/badany-tytul/food-service-polska/</t>
   </si>
   <si>
     <t>https://www.pbc.pl/badany-tytul/zawodarchitekt/</t>
@@ -1307,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,8 +1420,8 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>170</v>
+      <c r="B15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1441,7 +1429,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1449,7 +1437,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1465,7 +1453,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1473,7 +1461,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1481,7 +1469,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1489,7 +1477,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1497,7 +1485,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1505,7 +1493,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1513,7 +1501,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1521,7 +1509,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1529,7 +1517,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1537,7 +1525,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1545,12 +1533,12 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -1561,7 +1549,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1569,7 +1557,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1577,7 +1565,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1585,7 +1573,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1593,7 +1581,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1601,7 +1589,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1609,7 +1597,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1617,7 +1605,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1625,7 +1613,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1633,7 +1621,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1641,7 +1629,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1649,7 +1637,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1657,7 +1645,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1665,7 +1653,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1673,7 +1661,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1681,7 +1669,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1689,7 +1677,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1697,7 +1685,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1705,7 +1693,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1713,7 +1701,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1721,7 +1709,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1729,7 +1717,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1737,7 +1725,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1745,7 +1733,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1753,7 +1741,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1761,7 +1749,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1769,15 +1757,15 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>210</v>
+      <c r="B58" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1785,7 +1773,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1793,7 +1781,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1801,7 +1789,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1809,7 +1797,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1817,7 +1805,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1825,7 +1813,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1833,7 +1821,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1841,7 +1829,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1849,7 +1837,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1857,7 +1845,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1865,7 +1853,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1873,7 +1861,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1881,7 +1869,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1889,7 +1877,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1897,7 +1885,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1905,7 +1893,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1913,7 +1901,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1921,7 +1909,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1929,7 +1917,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1937,7 +1925,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1945,7 +1933,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1953,7 +1941,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1961,7 +1949,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1969,7 +1957,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1977,7 +1965,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1985,7 +1973,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1993,7 +1981,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -2001,7 +1989,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -2009,7 +1997,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -2017,7 +2005,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -2025,7 +2013,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -2033,15 +2021,15 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>242</v>
+      <c r="B91" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -2049,7 +2037,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -2057,7 +2045,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -2065,7 +2053,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -2073,7 +2061,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -2081,7 +2069,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -2089,7 +2077,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -2097,7 +2085,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -2105,7 +2093,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -2113,7 +2101,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2121,7 +2109,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2129,7 +2117,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -2137,15 +2125,15 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>254</v>
+      <c r="B104" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -2153,7 +2141,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2161,7 +2149,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -2169,7 +2157,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2177,7 +2165,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2185,7 +2173,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -2193,7 +2181,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -2201,7 +2189,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2209,7 +2197,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -2217,7 +2205,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2225,7 +2213,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -2233,7 +2221,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -2241,7 +2229,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -2249,7 +2237,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -2257,7 +2245,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -2265,7 +2253,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -2273,7 +2261,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -2281,7 +2269,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -2289,7 +2277,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -2297,7 +2285,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -2305,7 +2293,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -2313,7 +2301,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -2321,7 +2309,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -2329,7 +2317,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -2337,7 +2325,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -2345,7 +2333,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -2353,7 +2341,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -2361,7 +2349,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -2369,7 +2357,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -2377,7 +2365,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -2385,7 +2373,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -2393,7 +2381,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -2401,7 +2389,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -2409,7 +2397,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -2417,7 +2405,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -2425,7 +2413,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -2433,7 +2421,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -2441,7 +2429,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -2449,7 +2437,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
@@ -2465,7 +2453,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -2473,7 +2461,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -2481,7 +2469,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -2489,7 +2477,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -2497,7 +2485,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -2505,7 +2493,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -2521,7 +2509,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -2529,7 +2517,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -2537,7 +2525,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -2545,7 +2533,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -2553,7 +2541,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -2561,15 +2549,15 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2587,145 +2575,141 @@
     <hyperlink ref="B13" r:id="rId11" xr:uid="{CDD4AF71-1BF5-4B03-B1B5-AF057861AD3A}"/>
     <hyperlink ref="B12" r:id="rId12" xr:uid="{1EF7ADEC-39CC-44E4-B5D4-89FC268BE327}"/>
     <hyperlink ref="B14" r:id="rId13" xr:uid="{245679D0-CF22-426E-8C21-F25874C32783}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{A82340C1-3780-4A44-BE7F-AE72BF470B1D}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{901E09B6-C765-47F5-8EBF-96BEE320EC9F}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{8EFB89BF-84B4-406C-B571-932552DE4F97}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{889CD3C6-1A4F-4BD2-B12E-C97B3A871BCD}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{B3C84FE3-C8F1-46E5-B3E4-261D82B35081}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{0913F344-3177-4C15-8429-26B436E087FB}"/>
-    <hyperlink ref="B22" r:id="rId20" xr:uid="{C9BBB2FA-8E45-484E-993E-378BF9D67BED}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{43E1C270-A36B-4F56-AA26-63A949A0FB86}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{AC6940B2-7E6B-405A-901D-71884A33F6E8}"/>
-    <hyperlink ref="B25" r:id="rId23" xr:uid="{89EFE93A-C1D5-4181-A94C-1591A70D30F0}"/>
-    <hyperlink ref="B26" r:id="rId24" xr:uid="{AA27FF02-AA7D-45E2-ACA1-FFCA85054BB1}"/>
-    <hyperlink ref="B27" r:id="rId25" xr:uid="{6E34AEEA-3859-44A9-B86E-360DB14EC589}"/>
-    <hyperlink ref="B28" r:id="rId26" xr:uid="{00C8B8EE-E1C4-4F89-9E27-825CF827BBBB}"/>
-    <hyperlink ref="B29" r:id="rId27" xr:uid="{EDB1554D-EEDE-4111-98E4-C89EA0AB35A8}"/>
-    <hyperlink ref="B31" r:id="rId28" xr:uid="{1A074F19-C2A9-494C-BFAF-9EA1F42D46E9}"/>
-    <hyperlink ref="B32" r:id="rId29" xr:uid="{B8D910FB-DCCA-48B2-A43F-6B606FC00B2C}"/>
-    <hyperlink ref="B33" r:id="rId30" xr:uid="{C7E0BEBB-9B8C-4DFB-A188-DEFFE96535AA}"/>
-    <hyperlink ref="B34" r:id="rId31" xr:uid="{D317D14C-FA06-4B9E-9D0F-BCCD907084DA}"/>
-    <hyperlink ref="B35" r:id="rId32" xr:uid="{ADDAF22E-C0F8-413F-A607-FA7141B001E4}"/>
-    <hyperlink ref="B36" r:id="rId33" xr:uid="{D5DFBE68-B9AC-41EC-B990-C66131F80F63}"/>
-    <hyperlink ref="B37" r:id="rId34" xr:uid="{88623E8E-0E4E-47A3-A469-F0D3A6F9547A}"/>
-    <hyperlink ref="B38" r:id="rId35" xr:uid="{A7611018-7999-48D6-B81A-EB9C83902617}"/>
-    <hyperlink ref="B39" r:id="rId36" xr:uid="{42131F9A-978E-4AE7-B1D9-E0C41DD573B9}"/>
-    <hyperlink ref="B40" r:id="rId37" xr:uid="{C8431CEC-22B3-43EE-9FCD-51D6AC361A54}"/>
-    <hyperlink ref="B41" r:id="rId38" xr:uid="{4D2F4DD3-5C82-4DC5-9C77-82C1D50C4E0E}"/>
-    <hyperlink ref="B42" r:id="rId39" xr:uid="{8B51195B-77D3-4A35-B95E-0D457D733A24}"/>
-    <hyperlink ref="B43" r:id="rId40" xr:uid="{804F721E-A6AE-488B-98E5-B749E6D20561}"/>
-    <hyperlink ref="B44" r:id="rId41" xr:uid="{C24BF185-82A8-4065-93F6-931AFF9B03DC}"/>
-    <hyperlink ref="B45" r:id="rId42" xr:uid="{C67B7094-E170-4B52-858E-006C94E8EA5F}"/>
-    <hyperlink ref="B46" r:id="rId43" xr:uid="{5ECEE0FB-ED7E-4AF9-8AF3-7E9FA3CD9132}"/>
-    <hyperlink ref="B47" r:id="rId44" xr:uid="{2A4FE03F-CEAD-4454-8B20-673BC299AB03}"/>
-    <hyperlink ref="B48" r:id="rId45" xr:uid="{E280DAB2-145E-4B12-BDF1-24CACFD10985}"/>
-    <hyperlink ref="B49" r:id="rId46" xr:uid="{44C6C2BA-6FE8-4F3F-B0DA-DE1839A996EB}"/>
-    <hyperlink ref="B50" r:id="rId47" xr:uid="{BA328256-F882-442E-9201-48005E2D1131}"/>
-    <hyperlink ref="B51" r:id="rId48" xr:uid="{420E7AEA-4805-4BFB-A26F-E1F214BA25A2}"/>
-    <hyperlink ref="B52" r:id="rId49" xr:uid="{26CEEF05-D319-4E23-B3DA-B659A6AD6EEA}"/>
-    <hyperlink ref="B53" r:id="rId50" xr:uid="{FE156699-9D1E-4336-AF49-FF2D5C005330}"/>
-    <hyperlink ref="B54" r:id="rId51" xr:uid="{7AAE087E-3EB9-4657-984D-C50FCF78F725}"/>
-    <hyperlink ref="B55" r:id="rId52" xr:uid="{E94FC155-2278-4E0A-8D6A-057F088DF1E9}"/>
-    <hyperlink ref="B56" r:id="rId53" xr:uid="{17BB482F-923B-4C5D-8B34-62D1BC3FA8D2}"/>
-    <hyperlink ref="B57" r:id="rId54" xr:uid="{B79C568C-BC56-4F68-8A0B-DD5CF125D8CD}"/>
-    <hyperlink ref="B58" r:id="rId55" xr:uid="{2491AF29-CF7D-4488-B632-375463716AA9}"/>
-    <hyperlink ref="B59" r:id="rId56" xr:uid="{12276849-ADAC-496A-BA1D-A8E3BE46A41C}"/>
-    <hyperlink ref="B60" r:id="rId57" xr:uid="{EFEAC5CA-F874-4946-87CD-EA21A96DE2C0}"/>
-    <hyperlink ref="B61" r:id="rId58" xr:uid="{2A363481-3080-44C5-80FA-6A71F96FA662}"/>
-    <hyperlink ref="B62" r:id="rId59" xr:uid="{9D7F5C8B-1D38-46BE-9A0D-8BF47CDF5421}"/>
-    <hyperlink ref="B63" r:id="rId60" xr:uid="{EB0DDAB1-65F4-4E68-AE75-9F038B858258}"/>
-    <hyperlink ref="B64" r:id="rId61" xr:uid="{56CBBAAB-5068-43A6-82B7-F1B2D36AB7F0}"/>
-    <hyperlink ref="B65" r:id="rId62" xr:uid="{DF6D625C-CA9C-4FD3-8272-F867EB93261A}"/>
-    <hyperlink ref="B66" r:id="rId63" xr:uid="{E1336EF5-5485-4079-A4B6-88D86CF3F7F8}"/>
-    <hyperlink ref="B67" r:id="rId64" xr:uid="{77DF8C44-6377-4634-9CB0-3741A3BEDECE}"/>
-    <hyperlink ref="B68" r:id="rId65" xr:uid="{EE7C015E-6FE3-4AE3-AC94-EE8F6830FC18}"/>
-    <hyperlink ref="B70" r:id="rId66" xr:uid="{B6509F81-5722-424D-864B-AFF831FA892F}"/>
-    <hyperlink ref="B71" r:id="rId67" xr:uid="{980F04C9-2080-4B69-8E49-1AF29D9E35C4}"/>
-    <hyperlink ref="B72" r:id="rId68" xr:uid="{1710E8A9-9BC3-4526-8D76-B86F2A233FE1}"/>
-    <hyperlink ref="B73" r:id="rId69" xr:uid="{4D52220B-3359-41C7-8C81-E7CB2E95F7FB}"/>
-    <hyperlink ref="B74" r:id="rId70" xr:uid="{4974557C-062C-4D7E-A195-F2E37DEE1374}"/>
-    <hyperlink ref="B75" r:id="rId71" xr:uid="{54B6DF49-401B-4BCA-BE50-6E798BA92C55}"/>
-    <hyperlink ref="B76" r:id="rId72" xr:uid="{1EAD05C9-AAF5-47BF-8DC3-F8E795863659}"/>
-    <hyperlink ref="B77" r:id="rId73" xr:uid="{DC75F25A-DB25-4E8D-A257-C924D1A36A5D}"/>
-    <hyperlink ref="B78" r:id="rId74" xr:uid="{B0F31FBF-94BC-49EA-99EC-8703A9415DD7}"/>
-    <hyperlink ref="B79" r:id="rId75" xr:uid="{1FCE2DE9-2C8F-4BE1-B8EC-7BC863081FB5}"/>
-    <hyperlink ref="B80" r:id="rId76" xr:uid="{C5EDDD38-3797-484A-BBB8-FFFFD9926F8E}"/>
-    <hyperlink ref="B81" r:id="rId77" xr:uid="{DAF9B1B8-D83D-4B59-8E7A-F0BCE3C8552D}"/>
-    <hyperlink ref="B82" r:id="rId78" xr:uid="{BB877012-6EBD-4568-9338-1986550697F0}"/>
-    <hyperlink ref="B83" r:id="rId79" xr:uid="{AC0FD1FE-52EA-4468-960C-C509CAB849BF}"/>
-    <hyperlink ref="B84" r:id="rId80" xr:uid="{7C49C1A4-2E40-44D1-B42F-4BE985F7CF4C}"/>
-    <hyperlink ref="B85" r:id="rId81" xr:uid="{8A2F77C0-090F-4785-927D-CD918C094A3F}"/>
-    <hyperlink ref="B86" r:id="rId82" xr:uid="{44C5B551-4E5A-400E-B933-38AF8DE156E0}"/>
-    <hyperlink ref="B87" r:id="rId83" xr:uid="{264F9B6A-046E-4970-B81D-3E8979AB3ABA}"/>
-    <hyperlink ref="B88" r:id="rId84" xr:uid="{BAE0E03F-9EB5-409D-90E6-5A95D8076283}"/>
-    <hyperlink ref="B89" r:id="rId85" xr:uid="{DD8B9EA1-FFC4-4F2F-8754-ED30DAC404E0}"/>
-    <hyperlink ref="B90" r:id="rId86" xr:uid="{97E1B4F2-3690-4AE9-BEDE-585B80A211EF}"/>
-    <hyperlink ref="B91" r:id="rId87" xr:uid="{9B554312-3276-4187-B25B-CAF62C687E9A}"/>
-    <hyperlink ref="B92" r:id="rId88" xr:uid="{6D3FCE3F-AD29-47BC-A20B-BE0C14FDE18E}"/>
-    <hyperlink ref="B93" r:id="rId89" xr:uid="{F2D90CE7-FF9D-4FF5-84C2-DF83C02B4CD3}"/>
-    <hyperlink ref="B94" r:id="rId90" xr:uid="{F838C6B1-DDA7-45F7-84F5-07A436DEA6BD}"/>
-    <hyperlink ref="B95" r:id="rId91" xr:uid="{7154537B-B079-4116-8125-C43DCF28B2A5}"/>
-    <hyperlink ref="B96" r:id="rId92" xr:uid="{881F1050-C89C-4820-9766-A688AE96E328}"/>
-    <hyperlink ref="B97" r:id="rId93" xr:uid="{091FC7F8-F4E1-4057-BE9C-1B3A08D6A303}"/>
-    <hyperlink ref="B98" r:id="rId94" xr:uid="{FF5D30B6-9733-4DDD-8F08-605BEDB65869}"/>
-    <hyperlink ref="B99" r:id="rId95" xr:uid="{A0471D2B-9E17-4A61-9749-E3AF9230D282}"/>
-    <hyperlink ref="B100" r:id="rId96" xr:uid="{32EC803D-FE57-491E-BFBD-627C81311EB9}"/>
-    <hyperlink ref="B101" r:id="rId97" xr:uid="{29EA50BF-D5FA-476C-957E-9936E6A97F32}"/>
-    <hyperlink ref="B102" r:id="rId98" xr:uid="{C778AFB2-0F7D-4C15-BEBE-8C2ACBACE9EC}"/>
-    <hyperlink ref="B103" r:id="rId99" xr:uid="{FEA6C35B-ED89-4801-A5E3-B0CA99010251}"/>
-    <hyperlink ref="B104" r:id="rId100" xr:uid="{6A7DD783-B53C-44A7-923B-FAD76B79CD23}"/>
-    <hyperlink ref="B105" r:id="rId101" xr:uid="{D21D2FC7-659E-4162-A2F8-109A2B4A59D8}"/>
-    <hyperlink ref="B106" r:id="rId102" xr:uid="{A3D141C8-B260-4916-BA94-1A908DA68CD3}"/>
-    <hyperlink ref="B107" r:id="rId103" xr:uid="{15250B50-5F15-473C-9C9A-A2AA0F324336}"/>
-    <hyperlink ref="B108" r:id="rId104" xr:uid="{A4A25588-7E24-49C2-B9C0-BF031E691C72}"/>
-    <hyperlink ref="B109" r:id="rId105" xr:uid="{4A7D46B3-AC36-48C6-9263-97E7C718C4B4}"/>
-    <hyperlink ref="B110" r:id="rId106" xr:uid="{53209B30-B0BE-4C83-977B-D04F756D6D0D}"/>
-    <hyperlink ref="B111" r:id="rId107" xr:uid="{AA5B7810-3C61-4368-9B43-B5F1E2FABED6}"/>
-    <hyperlink ref="B112" r:id="rId108" xr:uid="{30BAE52B-5BF6-498E-BCEB-550E258A1A87}"/>
-    <hyperlink ref="B113" r:id="rId109" xr:uid="{DF6CCC45-1AEC-49C4-8A3E-48F0DEBE035B}"/>
-    <hyperlink ref="B114" r:id="rId110" xr:uid="{D853F143-8E45-40DA-818C-B2E7D942BDBE}"/>
-    <hyperlink ref="B115" r:id="rId111" xr:uid="{A60530A3-BF52-42A6-BCF5-00A24CC8FC09}"/>
-    <hyperlink ref="B116" r:id="rId112" xr:uid="{80EDD1B5-D0E9-47A9-BB36-553F253035BE}"/>
-    <hyperlink ref="B117" r:id="rId113" xr:uid="{A3DC3AB7-9840-419F-8483-66367B99B782}"/>
-    <hyperlink ref="B118" r:id="rId114" xr:uid="{3A051F18-EE40-45A5-9A69-EEFFD1120AC1}"/>
-    <hyperlink ref="B119" r:id="rId115" xr:uid="{C9A56A4D-95CB-4F0A-A838-C20AAE1707CD}"/>
-    <hyperlink ref="B120" r:id="rId116" xr:uid="{C4F14C55-0CE1-4D5A-8232-643A7D555729}"/>
-    <hyperlink ref="B121" r:id="rId117" xr:uid="{9B074018-6501-4CB1-AEBF-5FBFACCC02D0}"/>
-    <hyperlink ref="B122" r:id="rId118" xr:uid="{598A1FD0-5A29-4D4C-8976-1F5428808AE2}"/>
-    <hyperlink ref="B123" r:id="rId119" xr:uid="{A3351596-6352-4A99-9D44-ECA073050931}"/>
-    <hyperlink ref="B124" r:id="rId120" xr:uid="{20305582-44C4-4D24-BA60-58B78ACC3317}"/>
-    <hyperlink ref="B125" r:id="rId121" xr:uid="{AAE31A2E-A547-443C-815B-0F0CC125622D}"/>
-    <hyperlink ref="B126" r:id="rId122" xr:uid="{2983F601-F621-4AE3-9E7B-5C444351E683}"/>
-    <hyperlink ref="B127" r:id="rId123" xr:uid="{B09DE008-E814-409F-BA48-8C5AFEE0DCB7}"/>
-    <hyperlink ref="B128" r:id="rId124" xr:uid="{634A88D0-EE85-4185-BA9F-C87EC69DB7D8}"/>
-    <hyperlink ref="B129" r:id="rId125" xr:uid="{8BF48175-A232-48EB-8FCB-FA91BE1E48FD}"/>
-    <hyperlink ref="B130" r:id="rId126" xr:uid="{CB89FA8A-716D-450B-B08D-D619AF5B8ED3}"/>
-    <hyperlink ref="B131" r:id="rId127" xr:uid="{DC001BBB-E130-4FD8-B8CB-5FBAB26525CC}"/>
-    <hyperlink ref="B132" r:id="rId128" xr:uid="{6960E9F2-75A6-4C5C-8B0A-9BB42C095587}"/>
-    <hyperlink ref="B133" r:id="rId129" xr:uid="{C371067F-F96F-40DC-9150-2C176FF77B4D}"/>
-    <hyperlink ref="B134" r:id="rId130" xr:uid="{BA9C23AD-D005-4C22-B97F-74A57DA0EA44}"/>
-    <hyperlink ref="B135" r:id="rId131" xr:uid="{06B12A1D-1C4D-4DE4-BB8B-2FA12F66494B}"/>
-    <hyperlink ref="B136" r:id="rId132" xr:uid="{ED6BB2DE-333E-4240-9D4B-79BFEEFD4C94}"/>
-    <hyperlink ref="B137" r:id="rId133" xr:uid="{DF803BFB-2FB0-42E7-BB0F-F8B8AE7419D0}"/>
-    <hyperlink ref="B138" r:id="rId134" xr:uid="{EDE28C73-D9CC-470C-A7D8-B2B3F0E310EF}"/>
-    <hyperlink ref="B139" r:id="rId135" xr:uid="{EB9D5654-E1E6-4A42-9010-A0EFF9500584}"/>
-    <hyperlink ref="B140" r:id="rId136" xr:uid="{C30CB670-D192-466E-98FE-131CEDCD24CA}"/>
-    <hyperlink ref="B141" r:id="rId137" xr:uid="{99EA9DC8-AAA0-47AC-8071-56532CEF90FC}"/>
-    <hyperlink ref="B142" r:id="rId138" xr:uid="{20D2189B-C2CB-4193-A168-E164603F7EC4}"/>
-    <hyperlink ref="B144" r:id="rId139" xr:uid="{5C558677-FB03-478D-AD1B-4FFCCC115FE2}"/>
-    <hyperlink ref="B145" r:id="rId140" xr:uid="{53E5CF2F-BD5B-4804-96CD-06D1B79B792B}"/>
-    <hyperlink ref="B146" r:id="rId141" xr:uid="{FEDC7E2D-9615-4F18-A1AC-D03A5891BF66}"/>
-    <hyperlink ref="B147" r:id="rId142" xr:uid="{391DAA67-11D1-48EE-B715-D3D65C5E92D5}"/>
-    <hyperlink ref="B148" r:id="rId143" xr:uid="{9088089A-1B54-4158-BED5-E99692A51DC5}"/>
-    <hyperlink ref="B149" r:id="rId144" xr:uid="{5DA818E4-EBE4-45A5-BAB6-99AC0F62F52E}"/>
-    <hyperlink ref="B151" r:id="rId145" xr:uid="{A371E8FF-CA6F-474C-8B6C-991EE5EAB867}"/>
-    <hyperlink ref="B152" r:id="rId146" xr:uid="{0EBF07EA-25F2-4EF4-8D4D-F56177C03BC6}"/>
-    <hyperlink ref="B153" r:id="rId147" xr:uid="{F7AD252C-ECF4-44AA-880F-EF9D9A0E9862}"/>
-    <hyperlink ref="B154" r:id="rId148" xr:uid="{B1F2C660-EB56-49F4-95CD-AA2BA5B3F7D5}"/>
-    <hyperlink ref="B155" r:id="rId149" xr:uid="{34AD9BF7-6D50-4D79-82E7-F6982D4296DD}"/>
-    <hyperlink ref="B156" r:id="rId150" xr:uid="{B21D8D1E-65CF-446F-9AFF-AAEEF461ADFB}"/>
-    <hyperlink ref="B69" r:id="rId151" xr:uid="{97DF5C80-E005-40AB-BEDC-3AC7500D05F5}"/>
-    <hyperlink ref="B157" r:id="rId152" xr:uid="{1A8D4925-4BC9-46BC-BF5B-1DCC68AA8D79}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{901E09B6-C765-47F5-8EBF-96BEE320EC9F}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{8EFB89BF-84B4-406C-B571-932552DE4F97}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{889CD3C6-1A4F-4BD2-B12E-C97B3A871BCD}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{B3C84FE3-C8F1-46E5-B3E4-261D82B35081}"/>
+    <hyperlink ref="B21" r:id="rId18" xr:uid="{0913F344-3177-4C15-8429-26B436E087FB}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{C9BBB2FA-8E45-484E-993E-378BF9D67BED}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{43E1C270-A36B-4F56-AA26-63A949A0FB86}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{AC6940B2-7E6B-405A-901D-71884A33F6E8}"/>
+    <hyperlink ref="B25" r:id="rId22" xr:uid="{89EFE93A-C1D5-4181-A94C-1591A70D30F0}"/>
+    <hyperlink ref="B26" r:id="rId23" xr:uid="{AA27FF02-AA7D-45E2-ACA1-FFCA85054BB1}"/>
+    <hyperlink ref="B27" r:id="rId24" xr:uid="{6E34AEEA-3859-44A9-B86E-360DB14EC589}"/>
+    <hyperlink ref="B28" r:id="rId25" xr:uid="{00C8B8EE-E1C4-4F89-9E27-825CF827BBBB}"/>
+    <hyperlink ref="B29" r:id="rId26" xr:uid="{EDB1554D-EEDE-4111-98E4-C89EA0AB35A8}"/>
+    <hyperlink ref="B31" r:id="rId27" xr:uid="{1A074F19-C2A9-494C-BFAF-9EA1F42D46E9}"/>
+    <hyperlink ref="B32" r:id="rId28" xr:uid="{B8D910FB-DCCA-48B2-A43F-6B606FC00B2C}"/>
+    <hyperlink ref="B33" r:id="rId29" xr:uid="{C7E0BEBB-9B8C-4DFB-A188-DEFFE96535AA}"/>
+    <hyperlink ref="B34" r:id="rId30" xr:uid="{D317D14C-FA06-4B9E-9D0F-BCCD907084DA}"/>
+    <hyperlink ref="B35" r:id="rId31" xr:uid="{ADDAF22E-C0F8-413F-A607-FA7141B001E4}"/>
+    <hyperlink ref="B36" r:id="rId32" xr:uid="{D5DFBE68-B9AC-41EC-B990-C66131F80F63}"/>
+    <hyperlink ref="B37" r:id="rId33" xr:uid="{88623E8E-0E4E-47A3-A469-F0D3A6F9547A}"/>
+    <hyperlink ref="B38" r:id="rId34" xr:uid="{A7611018-7999-48D6-B81A-EB9C83902617}"/>
+    <hyperlink ref="B39" r:id="rId35" xr:uid="{42131F9A-978E-4AE7-B1D9-E0C41DD573B9}"/>
+    <hyperlink ref="B40" r:id="rId36" xr:uid="{C8431CEC-22B3-43EE-9FCD-51D6AC361A54}"/>
+    <hyperlink ref="B41" r:id="rId37" xr:uid="{4D2F4DD3-5C82-4DC5-9C77-82C1D50C4E0E}"/>
+    <hyperlink ref="B42" r:id="rId38" xr:uid="{8B51195B-77D3-4A35-B95E-0D457D733A24}"/>
+    <hyperlink ref="B43" r:id="rId39" xr:uid="{804F721E-A6AE-488B-98E5-B749E6D20561}"/>
+    <hyperlink ref="B44" r:id="rId40" xr:uid="{C24BF185-82A8-4065-93F6-931AFF9B03DC}"/>
+    <hyperlink ref="B45" r:id="rId41" xr:uid="{C67B7094-E170-4B52-858E-006C94E8EA5F}"/>
+    <hyperlink ref="B46" r:id="rId42" xr:uid="{5ECEE0FB-ED7E-4AF9-8AF3-7E9FA3CD9132}"/>
+    <hyperlink ref="B47" r:id="rId43" xr:uid="{2A4FE03F-CEAD-4454-8B20-673BC299AB03}"/>
+    <hyperlink ref="B48" r:id="rId44" xr:uid="{E280DAB2-145E-4B12-BDF1-24CACFD10985}"/>
+    <hyperlink ref="B49" r:id="rId45" xr:uid="{44C6C2BA-6FE8-4F3F-B0DA-DE1839A996EB}"/>
+    <hyperlink ref="B50" r:id="rId46" xr:uid="{BA328256-F882-442E-9201-48005E2D1131}"/>
+    <hyperlink ref="B51" r:id="rId47" xr:uid="{420E7AEA-4805-4BFB-A26F-E1F214BA25A2}"/>
+    <hyperlink ref="B52" r:id="rId48" xr:uid="{26CEEF05-D319-4E23-B3DA-B659A6AD6EEA}"/>
+    <hyperlink ref="B53" r:id="rId49" xr:uid="{FE156699-9D1E-4336-AF49-FF2D5C005330}"/>
+    <hyperlink ref="B54" r:id="rId50" xr:uid="{7AAE087E-3EB9-4657-984D-C50FCF78F725}"/>
+    <hyperlink ref="B55" r:id="rId51" xr:uid="{E94FC155-2278-4E0A-8D6A-057F088DF1E9}"/>
+    <hyperlink ref="B56" r:id="rId52" xr:uid="{17BB482F-923B-4C5D-8B34-62D1BC3FA8D2}"/>
+    <hyperlink ref="B57" r:id="rId53" xr:uid="{B79C568C-BC56-4F68-8A0B-DD5CF125D8CD}"/>
+    <hyperlink ref="B59" r:id="rId54" xr:uid="{12276849-ADAC-496A-BA1D-A8E3BE46A41C}"/>
+    <hyperlink ref="B60" r:id="rId55" xr:uid="{EFEAC5CA-F874-4946-87CD-EA21A96DE2C0}"/>
+    <hyperlink ref="B61" r:id="rId56" xr:uid="{2A363481-3080-44C5-80FA-6A71F96FA662}"/>
+    <hyperlink ref="B62" r:id="rId57" xr:uid="{9D7F5C8B-1D38-46BE-9A0D-8BF47CDF5421}"/>
+    <hyperlink ref="B63" r:id="rId58" xr:uid="{EB0DDAB1-65F4-4E68-AE75-9F038B858258}"/>
+    <hyperlink ref="B64" r:id="rId59" xr:uid="{56CBBAAB-5068-43A6-82B7-F1B2D36AB7F0}"/>
+    <hyperlink ref="B65" r:id="rId60" xr:uid="{DF6D625C-CA9C-4FD3-8272-F867EB93261A}"/>
+    <hyperlink ref="B66" r:id="rId61" xr:uid="{E1336EF5-5485-4079-A4B6-88D86CF3F7F8}"/>
+    <hyperlink ref="B67" r:id="rId62" xr:uid="{77DF8C44-6377-4634-9CB0-3741A3BEDECE}"/>
+    <hyperlink ref="B68" r:id="rId63" xr:uid="{EE7C015E-6FE3-4AE3-AC94-EE8F6830FC18}"/>
+    <hyperlink ref="B70" r:id="rId64" xr:uid="{B6509F81-5722-424D-864B-AFF831FA892F}"/>
+    <hyperlink ref="B71" r:id="rId65" xr:uid="{980F04C9-2080-4B69-8E49-1AF29D9E35C4}"/>
+    <hyperlink ref="B72" r:id="rId66" xr:uid="{1710E8A9-9BC3-4526-8D76-B86F2A233FE1}"/>
+    <hyperlink ref="B73" r:id="rId67" xr:uid="{4D52220B-3359-41C7-8C81-E7CB2E95F7FB}"/>
+    <hyperlink ref="B74" r:id="rId68" xr:uid="{4974557C-062C-4D7E-A195-F2E37DEE1374}"/>
+    <hyperlink ref="B75" r:id="rId69" xr:uid="{54B6DF49-401B-4BCA-BE50-6E798BA92C55}"/>
+    <hyperlink ref="B76" r:id="rId70" xr:uid="{1EAD05C9-AAF5-47BF-8DC3-F8E795863659}"/>
+    <hyperlink ref="B77" r:id="rId71" xr:uid="{DC75F25A-DB25-4E8D-A257-C924D1A36A5D}"/>
+    <hyperlink ref="B78" r:id="rId72" xr:uid="{B0F31FBF-94BC-49EA-99EC-8703A9415DD7}"/>
+    <hyperlink ref="B79" r:id="rId73" xr:uid="{1FCE2DE9-2C8F-4BE1-B8EC-7BC863081FB5}"/>
+    <hyperlink ref="B80" r:id="rId74" xr:uid="{C5EDDD38-3797-484A-BBB8-FFFFD9926F8E}"/>
+    <hyperlink ref="B81" r:id="rId75" xr:uid="{DAF9B1B8-D83D-4B59-8E7A-F0BCE3C8552D}"/>
+    <hyperlink ref="B82" r:id="rId76" xr:uid="{BB877012-6EBD-4568-9338-1986550697F0}"/>
+    <hyperlink ref="B83" r:id="rId77" xr:uid="{AC0FD1FE-52EA-4468-960C-C509CAB849BF}"/>
+    <hyperlink ref="B84" r:id="rId78" xr:uid="{7C49C1A4-2E40-44D1-B42F-4BE985F7CF4C}"/>
+    <hyperlink ref="B85" r:id="rId79" xr:uid="{8A2F77C0-090F-4785-927D-CD918C094A3F}"/>
+    <hyperlink ref="B86" r:id="rId80" xr:uid="{44C5B551-4E5A-400E-B933-38AF8DE156E0}"/>
+    <hyperlink ref="B87" r:id="rId81" xr:uid="{264F9B6A-046E-4970-B81D-3E8979AB3ABA}"/>
+    <hyperlink ref="B88" r:id="rId82" xr:uid="{BAE0E03F-9EB5-409D-90E6-5A95D8076283}"/>
+    <hyperlink ref="B89" r:id="rId83" xr:uid="{DD8B9EA1-FFC4-4F2F-8754-ED30DAC404E0}"/>
+    <hyperlink ref="B90" r:id="rId84" xr:uid="{97E1B4F2-3690-4AE9-BEDE-585B80A211EF}"/>
+    <hyperlink ref="B92" r:id="rId85" xr:uid="{6D3FCE3F-AD29-47BC-A20B-BE0C14FDE18E}"/>
+    <hyperlink ref="B93" r:id="rId86" xr:uid="{F2D90CE7-FF9D-4FF5-84C2-DF83C02B4CD3}"/>
+    <hyperlink ref="B94" r:id="rId87" xr:uid="{F838C6B1-DDA7-45F7-84F5-07A436DEA6BD}"/>
+    <hyperlink ref="B95" r:id="rId88" xr:uid="{7154537B-B079-4116-8125-C43DCF28B2A5}"/>
+    <hyperlink ref="B96" r:id="rId89" xr:uid="{881F1050-C89C-4820-9766-A688AE96E328}"/>
+    <hyperlink ref="B97" r:id="rId90" xr:uid="{091FC7F8-F4E1-4057-BE9C-1B3A08D6A303}"/>
+    <hyperlink ref="B98" r:id="rId91" xr:uid="{FF5D30B6-9733-4DDD-8F08-605BEDB65869}"/>
+    <hyperlink ref="B99" r:id="rId92" xr:uid="{A0471D2B-9E17-4A61-9749-E3AF9230D282}"/>
+    <hyperlink ref="B100" r:id="rId93" xr:uid="{32EC803D-FE57-491E-BFBD-627C81311EB9}"/>
+    <hyperlink ref="B101" r:id="rId94" xr:uid="{29EA50BF-D5FA-476C-957E-9936E6A97F32}"/>
+    <hyperlink ref="B102" r:id="rId95" xr:uid="{C778AFB2-0F7D-4C15-BEBE-8C2ACBACE9EC}"/>
+    <hyperlink ref="B103" r:id="rId96" xr:uid="{FEA6C35B-ED89-4801-A5E3-B0CA99010251}"/>
+    <hyperlink ref="B105" r:id="rId97" xr:uid="{D21D2FC7-659E-4162-A2F8-109A2B4A59D8}"/>
+    <hyperlink ref="B106" r:id="rId98" xr:uid="{A3D141C8-B260-4916-BA94-1A908DA68CD3}"/>
+    <hyperlink ref="B107" r:id="rId99" xr:uid="{15250B50-5F15-473C-9C9A-A2AA0F324336}"/>
+    <hyperlink ref="B108" r:id="rId100" xr:uid="{A4A25588-7E24-49C2-B9C0-BF031E691C72}"/>
+    <hyperlink ref="B109" r:id="rId101" xr:uid="{4A7D46B3-AC36-48C6-9263-97E7C718C4B4}"/>
+    <hyperlink ref="B110" r:id="rId102" xr:uid="{53209B30-B0BE-4C83-977B-D04F756D6D0D}"/>
+    <hyperlink ref="B111" r:id="rId103" xr:uid="{AA5B7810-3C61-4368-9B43-B5F1E2FABED6}"/>
+    <hyperlink ref="B112" r:id="rId104" xr:uid="{30BAE52B-5BF6-498E-BCEB-550E258A1A87}"/>
+    <hyperlink ref="B113" r:id="rId105" xr:uid="{DF6CCC45-1AEC-49C4-8A3E-48F0DEBE035B}"/>
+    <hyperlink ref="B114" r:id="rId106" xr:uid="{D853F143-8E45-40DA-818C-B2E7D942BDBE}"/>
+    <hyperlink ref="B115" r:id="rId107" xr:uid="{A60530A3-BF52-42A6-BCF5-00A24CC8FC09}"/>
+    <hyperlink ref="B116" r:id="rId108" xr:uid="{80EDD1B5-D0E9-47A9-BB36-553F253035BE}"/>
+    <hyperlink ref="B117" r:id="rId109" xr:uid="{A3DC3AB7-9840-419F-8483-66367B99B782}"/>
+    <hyperlink ref="B118" r:id="rId110" xr:uid="{3A051F18-EE40-45A5-9A69-EEFFD1120AC1}"/>
+    <hyperlink ref="B119" r:id="rId111" xr:uid="{C9A56A4D-95CB-4F0A-A838-C20AAE1707CD}"/>
+    <hyperlink ref="B120" r:id="rId112" xr:uid="{C4F14C55-0CE1-4D5A-8232-643A7D555729}"/>
+    <hyperlink ref="B121" r:id="rId113" xr:uid="{9B074018-6501-4CB1-AEBF-5FBFACCC02D0}"/>
+    <hyperlink ref="B122" r:id="rId114" xr:uid="{598A1FD0-5A29-4D4C-8976-1F5428808AE2}"/>
+    <hyperlink ref="B123" r:id="rId115" xr:uid="{A3351596-6352-4A99-9D44-ECA073050931}"/>
+    <hyperlink ref="B124" r:id="rId116" xr:uid="{20305582-44C4-4D24-BA60-58B78ACC3317}"/>
+    <hyperlink ref="B125" r:id="rId117" xr:uid="{AAE31A2E-A547-443C-815B-0F0CC125622D}"/>
+    <hyperlink ref="B126" r:id="rId118" xr:uid="{2983F601-F621-4AE3-9E7B-5C444351E683}"/>
+    <hyperlink ref="B127" r:id="rId119" xr:uid="{B09DE008-E814-409F-BA48-8C5AFEE0DCB7}"/>
+    <hyperlink ref="B128" r:id="rId120" xr:uid="{634A88D0-EE85-4185-BA9F-C87EC69DB7D8}"/>
+    <hyperlink ref="B129" r:id="rId121" xr:uid="{8BF48175-A232-48EB-8FCB-FA91BE1E48FD}"/>
+    <hyperlink ref="B130" r:id="rId122" xr:uid="{CB89FA8A-716D-450B-B08D-D619AF5B8ED3}"/>
+    <hyperlink ref="B131" r:id="rId123" xr:uid="{DC001BBB-E130-4FD8-B8CB-5FBAB26525CC}"/>
+    <hyperlink ref="B132" r:id="rId124" xr:uid="{6960E9F2-75A6-4C5C-8B0A-9BB42C095587}"/>
+    <hyperlink ref="B133" r:id="rId125" xr:uid="{C371067F-F96F-40DC-9150-2C176FF77B4D}"/>
+    <hyperlink ref="B134" r:id="rId126" xr:uid="{BA9C23AD-D005-4C22-B97F-74A57DA0EA44}"/>
+    <hyperlink ref="B135" r:id="rId127" xr:uid="{06B12A1D-1C4D-4DE4-BB8B-2FA12F66494B}"/>
+    <hyperlink ref="B136" r:id="rId128" xr:uid="{ED6BB2DE-333E-4240-9D4B-79BFEEFD4C94}"/>
+    <hyperlink ref="B137" r:id="rId129" xr:uid="{DF803BFB-2FB0-42E7-BB0F-F8B8AE7419D0}"/>
+    <hyperlink ref="B138" r:id="rId130" xr:uid="{EDE28C73-D9CC-470C-A7D8-B2B3F0E310EF}"/>
+    <hyperlink ref="B139" r:id="rId131" xr:uid="{EB9D5654-E1E6-4A42-9010-A0EFF9500584}"/>
+    <hyperlink ref="B140" r:id="rId132" xr:uid="{C30CB670-D192-466E-98FE-131CEDCD24CA}"/>
+    <hyperlink ref="B141" r:id="rId133" xr:uid="{99EA9DC8-AAA0-47AC-8071-56532CEF90FC}"/>
+    <hyperlink ref="B142" r:id="rId134" xr:uid="{20D2189B-C2CB-4193-A168-E164603F7EC4}"/>
+    <hyperlink ref="B144" r:id="rId135" xr:uid="{5C558677-FB03-478D-AD1B-4FFCCC115FE2}"/>
+    <hyperlink ref="B145" r:id="rId136" xr:uid="{53E5CF2F-BD5B-4804-96CD-06D1B79B792B}"/>
+    <hyperlink ref="B146" r:id="rId137" xr:uid="{FEDC7E2D-9615-4F18-A1AC-D03A5891BF66}"/>
+    <hyperlink ref="B147" r:id="rId138" xr:uid="{391DAA67-11D1-48EE-B715-D3D65C5E92D5}"/>
+    <hyperlink ref="B148" r:id="rId139" xr:uid="{9088089A-1B54-4158-BED5-E99692A51DC5}"/>
+    <hyperlink ref="B149" r:id="rId140" xr:uid="{5DA818E4-EBE4-45A5-BAB6-99AC0F62F52E}"/>
+    <hyperlink ref="B151" r:id="rId141" xr:uid="{A371E8FF-CA6F-474C-8B6C-991EE5EAB867}"/>
+    <hyperlink ref="B152" r:id="rId142" xr:uid="{0EBF07EA-25F2-4EF4-8D4D-F56177C03BC6}"/>
+    <hyperlink ref="B153" r:id="rId143" xr:uid="{F7AD252C-ECF4-44AA-880F-EF9D9A0E9862}"/>
+    <hyperlink ref="B154" r:id="rId144" xr:uid="{B1F2C660-EB56-49F4-95CD-AA2BA5B3F7D5}"/>
+    <hyperlink ref="B155" r:id="rId145" xr:uid="{34AD9BF7-6D50-4D79-82E7-F6982D4296DD}"/>
+    <hyperlink ref="B156" r:id="rId146" xr:uid="{B21D8D1E-65CF-446F-9AFF-AAEEF461ADFB}"/>
+    <hyperlink ref="B69" r:id="rId147" xr:uid="{97DF5C80-E005-40AB-BEDC-3AC7500D05F5}"/>
+    <hyperlink ref="B157" r:id="rId148" xr:uid="{1A8D4925-4BC9-46BC-BF5B-1DCC68AA8D79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>